<commit_message>
Feat: Implementar y depurar plataforma de castings funcional
</commit_message>
<xml_diff>
--- a/datos_modelos.xlsx
+++ b/datos_modelos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
   <si>
     <t>Nombre</t>
   </si>
@@ -99,6 +99,18 @@
   </si>
   <si>
     <t>valentina-rojas</t>
+  </si>
+  <si>
+    <t>Alba</t>
+  </si>
+  <si>
+    <t>Galocha</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>alba-galocha</t>
   </si>
   <si>
     <t>Pecho</t>
@@ -416,6 +428,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="13" width="17.63"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -538,6 +553,47 @@
       </c>
       <c r="M3" s="1" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="1">
+        <v>178.0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>88.0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>64.0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>92.0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>39.0</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -569,7 +625,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
@@ -595,13 +651,13 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D2" s="3">
         <v>185.0</v>
@@ -616,30 +672,30 @@
         <v>43.0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D3" s="3">
         <v>188.0</v>
@@ -657,16 +713,16 @@
         <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>